<commit_message>
The first 3 routes of the facility are working.
Added a few routes for the facility and almost done with the facility section.
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log-1_updated_bonus.xlsx
+++ b/DTT-Test-Hour-Log-1_updated_bonus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amberwessels/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\internship-dtt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49F91033-96F3-7148-A020-201798871A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A00F346-6DC2-407B-86DC-10F1F781A046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="500" windowWidth="34620" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -46,12 +46,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Example 1</t>
-  </si>
-  <si>
-    <t>Implementing …</t>
   </si>
   <si>
     <t>Example 2</t>
@@ -95,6 +89,12 @@
       <t xml:space="preserve"> 
 Fill in the number of hours that were required to complete the test. Please include every step you took during the process and include a detailed description of every step. Add reasoning on why you took certain decisions or applied specific techniques. We prefer quality over quantity so take your time with the test and the log.</t>
     </r>
+  </si>
+  <si>
+    <t>Start on the assignment</t>
+  </si>
+  <si>
+    <t>During this hour I oriënted myself for this assignment. First I read the assignment a few times to fully understand the requirements. After I was confident enough to start I read the Readme. The steps were easy to follow and creating the database scheme took a few minutes to determine which data types to use. After the setup of the database I wanted to know how to interact with the database so I can manipulate data. This was done very easily because the start-code already has a built-in database class. As a last step I set up the routes for the facility. The /facility route now returns all facilities with their corresponding tags. You can also create update and delete the facilities but I have not yet implemented the tags part in those routes.</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -447,6 +447,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1709,20 +1712,20 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.69921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.59765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.59765625" style="1" customWidth="1"/>
     <col min="5" max="6" width="6.5" style="1" customWidth="1"/>
     <col min="7" max="251" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1732,7 +1735,7 @@
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1740,7 +1743,7 @@
       <c r="E2" s="23"/>
       <c r="F2" s="24"/>
     </row>
-    <row r="3" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1754,29 +1757,29 @@
         <v>3</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B4" s="17">
-        <v>3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C4" s="18">
-        <v>42736</v>
+        <v>44729</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>5</v>
+      <c r="D4" s="25" t="s">
+        <v>13</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="17">
         <v>3</v>
@@ -1785,14 +1788,14 @@
         <v>42736</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="17">
         <v>5</v>
@@ -1801,14 +1804,14 @@
         <v>42736</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="17"/>
       <c r="C7" s="18"/>
@@ -1816,7 +1819,7 @@
       <c r="E7" s="20"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
@@ -1824,7 +1827,7 @@
       <c r="E8" s="20"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="17"/>
       <c r="C9" s="18"/>
@@ -1832,7 +1835,7 @@
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
@@ -1840,7 +1843,7 @@
       <c r="E10" s="20"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
@@ -1848,7 +1851,7 @@
       <c r="E11" s="20"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -1856,7 +1859,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="17"/>
       <c r="C13" s="18"/>
@@ -1864,7 +1867,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -1872,7 +1875,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -1880,7 +1883,7 @@
       <c r="E15" s="20"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -1888,7 +1891,7 @@
       <c r="E16" s="20"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -1896,7 +1899,7 @@
       <c r="E17" s="20"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
@@ -1904,7 +1907,7 @@
       <c r="E18" s="20"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="17"/>
       <c r="C19" s="18"/>
@@ -1912,7 +1915,7 @@
       <c r="E19" s="20"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -1920,7 +1923,7 @@
       <c r="E20" s="20"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
@@ -1928,7 +1931,7 @@
       <c r="E21" s="20"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="17"/>
       <c r="C22" s="18"/>
@@ -1936,7 +1939,7 @@
       <c r="E22" s="20"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
@@ -1944,7 +1947,7 @@
       <c r="E23" s="20"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
@@ -1952,7 +1955,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="17"/>
       <c r="C25" s="18"/>
@@ -1960,7 +1963,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
@@ -1968,7 +1971,7 @@
       <c r="E26" s="20"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="17"/>
       <c r="C27" s="18"/>
@@ -1976,7 +1979,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
@@ -1984,7 +1987,7 @@
       <c r="E28" s="20"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -1992,20 +1995,20 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2013,7 +2016,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2021,7 +2024,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>

</xml_diff>

<commit_message>
Imroved my code and updated hour log
Last week was not very productive for my assignment. During the week I work at my part time job. This is the company where I had my internship at the time of my MBO course. It was my intention to continue with the assignment on the Friday after work but instead I got sick. It was not Corona but a flu of some kind. Luckily for me, I have improved a lot in the last few days. During the last 2 days I have made some improvements to my application. I reflected on the way I handle errors. This could be done without the try catch method because this was a very cheap answer. To improve this I anticipated what parts of the code could give an error and tried to minimize the result. After the optimizations I am planning on implementing the bonus features. I have to keep in mind that it has already been a week since I’ve started on the assignment and that I should not take too much time.
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log-1_updated_bonus.xlsx
+++ b/DTT-Test-Hour-Log-1_updated_bonus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\internship-dtt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A00F346-6DC2-407B-86DC-10F1F781A046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C7E4AA-100B-41F8-BEF1-297B6D76722D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Subject</t>
   </si>
@@ -48,25 +48,10 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Example 2</t>
-  </si>
-  <si>
-    <t>Had some issues with…</t>
-  </si>
-  <si>
     <t>Total amount of hours</t>
   </si>
   <si>
     <t>Bonus</t>
-  </si>
-  <si>
-    <t>Example 3</t>
-  </si>
-  <si>
-    <t>Implemented bonus feature….</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <r>
@@ -95,6 +80,19 @@
   </si>
   <si>
     <t>During this hour I oriënted myself for this assignment. First I read the assignment a few times to fully understand the requirements. After I was confident enough to start I read the Readme. The steps were easy to follow and creating the database scheme took a few minutes to determine which data types to use. After the setup of the database I wanted to know how to interact with the database so I can manipulate data. This was done very easily because the start-code already has a built-in database class. As a last step I set up the routes for the facility. The /facility route now returns all facilities with their corresponding tags. You can also create update and delete the facilities but I have not yet implemented the tags part in those routes.</t>
+  </si>
+  <si>
+    <t>Working on the requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After working on the first route to fetch all the facilities, my understanding of rest API's had greatly improved. At first, I forgot to implement the tags of the facility. When the user called /facility, they got to see all the facilities but without their corresponding tags.  After this step, it was pretty easy to replicate the other CRUD routes. The POST was important because it had to be easy to use. The user should be able to create a facility with its tags and location. If the tags or location do not exist, they will be created. The PUT is also very important because this has to update the right facility along with it's tags. The DELETE route was pretty simple and straight forward. After getting the basics working, it was time to start on the filter method. I gave this a lot of thought but I think that the way I prepare my statements to build the query depending on the filter criteria is safe against SQL injections. Every input the user can give will be sanitized. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Last week was not very productive for my assignment. During the week I work at my part time job. This is the company where I had my internship at the time of my MBO course. It was my intention to continue with the assignment on the Friday after work but instead I got sick. It was not Corona but a flu of some kind. Luckily for me, I have improved a lot in the last few days. During the last 2 days I have made some improvements to my application. I reflected on the way I handle errors. This could be done without the try catch method because this was a very cheap answer. To improve this I anticipated what parts of the code could give an error and tried to minimize the result. After the optimizations I am planning on implementing the bonus features. I have to keep in mind that it has already been a week since I’ve started on the assignment and that I should not take too much time. </t>
+  </si>
+  <si>
+    <t>Improving my code</t>
   </si>
 </sst>
 </file>
@@ -397,7 +395,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -437,6 +435,12 @@
     <xf numFmtId="49" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -447,9 +451,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1712,7 +1713,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1726,24 +1727,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>11</v>
+      <c r="A2" s="25" t="s">
+        <v>6</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
@@ -1757,13 +1758,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" s="17">
         <v>1.1000000000000001</v>
@@ -1771,47 +1772,45 @@
       <c r="C4" s="18">
         <v>44729</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>13</v>
+      <c r="D4" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5" s="17">
-        <v>3</v>
+        <v>4.25</v>
       </c>
       <c r="C5" s="18">
-        <v>42736</v>
+        <v>44730</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>5</v>
+      <c r="D5" s="22" t="s">
+        <v>10</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" s="18">
-        <v>42736</v>
+        <v>44738</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>9</v>
+      <c r="D6" s="22" t="s">
+        <v>11</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="E6" s="20"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="17"/>
       <c r="C7" s="18"/>
@@ -1819,7 +1818,7 @@
       <c r="E7" s="20"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
@@ -1827,7 +1826,7 @@
       <c r="E8" s="20"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="17"/>
       <c r="C9" s="18"/>
@@ -1835,7 +1834,7 @@
       <c r="E9" s="20"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
@@ -1843,7 +1842,7 @@
       <c r="E10" s="20"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
@@ -1851,7 +1850,7 @@
       <c r="E11" s="20"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -1859,7 +1858,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="17"/>
       <c r="C13" s="18"/>
@@ -1867,7 +1866,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -1875,7 +1874,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -1883,7 +1882,7 @@
       <c r="E15" s="20"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -1891,7 +1890,7 @@
       <c r="E16" s="20"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -1899,7 +1898,7 @@
       <c r="E17" s="20"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
@@ -1907,7 +1906,7 @@
       <c r="E18" s="20"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="17"/>
       <c r="C19" s="18"/>
@@ -1915,7 +1914,7 @@
       <c r="E19" s="20"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -1923,7 +1922,7 @@
       <c r="E20" s="20"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
@@ -1931,7 +1930,7 @@
       <c r="E21" s="20"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="17"/>
       <c r="C22" s="18"/>
@@ -1939,7 +1938,7 @@
       <c r="E22" s="20"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
@@ -1947,7 +1946,7 @@
       <c r="E23" s="20"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18"/>
@@ -1955,7 +1954,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="17"/>
       <c r="C25" s="18"/>
@@ -1963,7 +1962,7 @@
       <c r="E25" s="20"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
@@ -1971,7 +1970,7 @@
       <c r="E26" s="20"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="17"/>
       <c r="C27" s="18"/>
@@ -1979,7 +1978,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
@@ -1987,7 +1986,7 @@
       <c r="E28" s="20"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -1995,13 +1994,13 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>4.0999999999999996</v>
+        <v>7.35</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>

</xml_diff>

<commit_message>
Cursor pagination + updated hour log + added SQL dump + added Enhanced entity-relationship diagram
I am not entirely sure about this but I think that I have implemented the cursor pagination. I have never implemented cursor pagination before so this was very new to me. First I started by researching what cursor pagination is. I followed many different courses and documentations. After a few minutes, I got a feeling that the concept was pretty clear to me. At that moment I started programming and searching online for different kinds of examples.
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log-1_updated_bonus.xlsx
+++ b/DTT-Test-Hour-Log-1_updated_bonus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\internship-dtt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C7E4AA-100B-41F8-BEF1-297B6D76722D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9D2C24-6867-42CC-AF2B-964F48E8B4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Subject</t>
   </si>
@@ -93,6 +93,21 @@
   </si>
   <si>
     <t>Improving my code</t>
+  </si>
+  <si>
+    <t>Today I wanted to work on the postman collection because this makes it easier to test. The routes are all explained as I thought needed. Some have more explanation than others but this is due to the difficulty of the route.</t>
+  </si>
+  <si>
+    <t>Making postman collection</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Implementing cursor pagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am not entirely sure about this but I think that I have implemented the cursor pagination. I have never implemented cursor pagination before so this was very new to me. First I started by researching what cursor pagination is. I followed many different courses, videos and documentations. After a few minutes I got the feeling that the concept was pretty clear to me. At that moment I started programming and searching online for different kinds of examples. </t>
   </si>
 </sst>
 </file>
@@ -1712,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1778,7 +1793,7 @@
       <c r="E4" s="20"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1794,7 +1809,7 @@
       <c r="E5" s="20"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>12</v>
       </c>
@@ -1810,23 +1825,43 @@
       <c r="E6" s="20"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="20"/>
+    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="17">
+        <v>1</v>
+      </c>
+      <c r="C7" s="18">
+        <v>44739</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="20"/>
+    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="17">
+        <v>1</v>
+      </c>
+      <c r="C8" s="18">
+        <v>44740</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="17"/>
       <c r="C9" s="18"/>

</xml_diff>